<commit_message>
channel proposal and Eval Cost
</commit_message>
<xml_diff>
--- a/input/Skeleton Output.xlsx
+++ b/input/Skeleton Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insidemedia-my.sharepoint.com/personal/sachin_saurav_groupm_com/Documents/one_pager_integration/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{7B35563C-D684-45BE-BEC8-21A80AD6596E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C39F2C27-05D0-4782-BCD3-B13CD4426792}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{7B35563C-D684-45BE-BEC8-21A80AD6596E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72115D25-A4CF-49C2-A7E9-A930B2517684}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1051,7 +1051,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1160,6 +1160,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="56">
     <border>
@@ -1861,7 +1867,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="309">
+  <cellXfs count="310">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2505,6 +2511,9 @@
     <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2593,6 +2602,97 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2601,107 +2701,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2709,8 +2718,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="2" fontId="28" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3061,32 +3070,32 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="226" t="s">
+      <c r="B2" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="227"/>
-      <c r="D2" s="227"/>
-      <c r="E2" s="227"/>
-      <c r="F2" s="227"/>
-      <c r="G2" s="227"/>
-      <c r="H2" s="227"/>
-      <c r="I2" s="227"/>
-      <c r="J2" s="227"/>
-      <c r="K2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="229"/>
     </row>
     <row r="3" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="233" t="s">
+      <c r="B3" s="234" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="234"/>
-      <c r="D3" s="234"/>
-      <c r="E3" s="234"/>
-      <c r="F3" s="234"/>
-      <c r="G3" s="234"/>
-      <c r="H3" s="234"/>
-      <c r="I3" s="234"/>
-      <c r="J3" s="234"/>
-      <c r="K3" s="235"/>
+      <c r="C3" s="235"/>
+      <c r="D3" s="235"/>
+      <c r="E3" s="235"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="235"/>
+      <c r="I3" s="235"/>
+      <c r="J3" s="235"/>
+      <c r="K3" s="236"/>
     </row>
     <row r="4" spans="2:11" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="141"/>
@@ -3502,10 +3511,10 @@
       <c r="C40" s="151" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="229" t="s">
+      <c r="D40" s="230" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="230"/>
+      <c r="E40" s="231"/>
       <c r="F40" s="172" t="s">
         <v>47</v>
       </c>
@@ -3516,11 +3525,11 @@
       <c r="C41" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="231">
+      <c r="D41" s="232">
         <f>'DBD One Pager-with Eval.'!D47</f>
         <v>0</v>
       </c>
-      <c r="E41" s="232"/>
+      <c r="E41" s="233"/>
       <c r="F41" s="188">
         <f>'DBD One Pager-with Eval.'!E47</f>
         <v>0</v>
@@ -3564,7 +3573,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="61" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D13" sqref="D13"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3591,34 +3600,34 @@
   <sheetData>
     <row r="1" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:16" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="236"/>
-      <c r="C2" s="237"/>
-      <c r="D2" s="237"/>
-      <c r="E2" s="237"/>
-      <c r="F2" s="237"/>
-      <c r="G2" s="237"/>
-      <c r="H2" s="237"/>
-      <c r="I2" s="237"/>
-      <c r="J2" s="237"/>
-      <c r="K2" s="237"/>
-      <c r="L2" s="237"/>
-      <c r="M2" s="237"/>
-      <c r="N2" s="237"/>
-      <c r="O2" s="237"/>
-      <c r="P2" s="238"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="238"/>
+      <c r="F2" s="238"/>
+      <c r="G2" s="238"/>
+      <c r="H2" s="238"/>
+      <c r="I2" s="238"/>
+      <c r="J2" s="238"/>
+      <c r="K2" s="238"/>
+      <c r="L2" s="238"/>
+      <c r="M2" s="238"/>
+      <c r="N2" s="238"/>
+      <c r="O2" s="238"/>
+      <c r="P2" s="239"/>
     </row>
     <row r="3" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="195"/>
       <c r="C3" s="196"/>
       <c r="D3" s="196"/>
-      <c r="E3" s="239" t="s">
+      <c r="E3" s="240" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="240"/>
-      <c r="G3" s="240"/>
-      <c r="H3" s="240"/>
-      <c r="I3" s="240"/>
-      <c r="J3" s="240"/>
+      <c r="F3" s="241"/>
+      <c r="G3" s="241"/>
+      <c r="H3" s="241"/>
+      <c r="I3" s="241"/>
+      <c r="J3" s="241"/>
       <c r="K3" s="196"/>
       <c r="L3" s="196"/>
       <c r="M3" s="197"/>
@@ -3634,20 +3643,20 @@
       <c r="B5" s="120">
         <v>1</v>
       </c>
-      <c r="C5" s="251"/>
-      <c r="D5" s="245"/>
-      <c r="E5" s="245"/>
-      <c r="F5" s="245"/>
-      <c r="G5" s="245"/>
-      <c r="H5" s="245"/>
-      <c r="I5" s="245"/>
-      <c r="J5" s="245"/>
+      <c r="C5" s="252"/>
+      <c r="D5" s="246"/>
+      <c r="E5" s="246"/>
+      <c r="F5" s="246"/>
+      <c r="G5" s="246"/>
+      <c r="H5" s="246"/>
+      <c r="I5" s="246"/>
+      <c r="J5" s="246"/>
       <c r="K5" s="199"/>
-      <c r="L5" s="259"/>
-      <c r="M5" s="245"/>
-      <c r="N5" s="245"/>
-      <c r="O5" s="245"/>
-      <c r="P5" s="260"/>
+      <c r="L5" s="260"/>
+      <c r="M5" s="246"/>
+      <c r="N5" s="246"/>
+      <c r="O5" s="246"/>
+      <c r="P5" s="261"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="120"/>
@@ -3665,12 +3674,12 @@
       <c r="B8" s="120">
         <v>2</v>
       </c>
-      <c r="C8" s="262" t="s">
+      <c r="C8" s="263" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="263"/>
-      <c r="E8" s="263"/>
-      <c r="F8" s="232"/>
+      <c r="D8" s="264"/>
+      <c r="E8" s="264"/>
+      <c r="F8" s="233"/>
       <c r="P8" s="123"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.35">
@@ -3798,9 +3807,9 @@
       <c r="F21" s="121"/>
       <c r="G21" s="152"/>
       <c r="H21" s="153"/>
-      <c r="I21" s="255"/>
-      <c r="J21" s="245"/>
-      <c r="K21" s="245"/>
+      <c r="I21" s="256"/>
+      <c r="J21" s="246"/>
+      <c r="K21" s="246"/>
       <c r="P21" s="123"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.35">
@@ -3811,9 +3820,9 @@
       <c r="F22" s="121"/>
       <c r="G22" s="152"/>
       <c r="H22" s="153"/>
-      <c r="I22" s="256"/>
-      <c r="J22" s="245"/>
-      <c r="K22" s="245"/>
+      <c r="I22" s="257"/>
+      <c r="J22" s="246"/>
+      <c r="K22" s="246"/>
       <c r="P22" s="123"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.35">
@@ -3824,10 +3833,10 @@
       <c r="B24" s="120">
         <v>5</v>
       </c>
-      <c r="C24" s="261" t="s">
+      <c r="C24" s="262" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="245"/>
+      <c r="D24" s="246"/>
       <c r="P24" s="123"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.35">
@@ -3843,15 +3852,15 @@
         <v>63</v>
       </c>
       <c r="E26" s="214"/>
-      <c r="K26" s="257" t="s">
+      <c r="K26" s="258" t="s">
         <v>64</v>
       </c>
-      <c r="L26" s="258"/>
-      <c r="M26" s="246" t="s">
+      <c r="L26" s="259"/>
+      <c r="M26" s="247" t="s">
         <v>65</v>
       </c>
-      <c r="N26" s="247"/>
-      <c r="O26" s="232"/>
+      <c r="N26" s="248"/>
+      <c r="O26" s="233"/>
       <c r="P26" s="123"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.35">
@@ -3912,15 +3921,15 @@
         <f>I28*G28/10</f>
         <v>0</v>
       </c>
-      <c r="K28" s="252" t="e">
+      <c r="K28" s="253" t="e">
         <f>L32/G32*10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L28" s="252"/>
+      <c r="L28" s="253"/>
       <c r="M28" s="221"/>
       <c r="N28" s="137"/>
       <c r="O28" s="134"/>
-      <c r="P28" s="248" t="s">
+      <c r="P28" s="249" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3937,12 +3946,12 @@
         <f>I29*G29/10</f>
         <v>0</v>
       </c>
-      <c r="K29" s="253"/>
-      <c r="L29" s="253"/>
+      <c r="K29" s="254"/>
+      <c r="L29" s="254"/>
       <c r="M29" s="221"/>
       <c r="N29" s="137"/>
       <c r="O29" s="134"/>
-      <c r="P29" s="249"/>
+      <c r="P29" s="250"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B30" s="120"/>
@@ -3957,12 +3966,12 @@
         <f>I30*G30/10</f>
         <v>0</v>
       </c>
-      <c r="K30" s="253"/>
-      <c r="L30" s="253"/>
+      <c r="K30" s="254"/>
+      <c r="L30" s="254"/>
       <c r="M30" s="221"/>
       <c r="N30" s="137"/>
       <c r="O30" s="134"/>
-      <c r="P30" s="249"/>
+      <c r="P30" s="250"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B31" s="120"/>
@@ -3977,12 +3986,12 @@
         <f>I31*G31/10</f>
         <v>0</v>
       </c>
-      <c r="K31" s="254"/>
-      <c r="L31" s="254"/>
+      <c r="K31" s="255"/>
+      <c r="L31" s="255"/>
       <c r="M31" s="221"/>
       <c r="N31" s="137"/>
       <c r="O31" s="134"/>
-      <c r="P31" s="250"/>
+      <c r="P31" s="251"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B32" s="120"/>
@@ -4076,22 +4085,22 @@
       <c r="B35" s="120">
         <v>7</v>
       </c>
-      <c r="C35" s="244" t="s">
+      <c r="C35" s="245" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="245"/>
+      <c r="D35" s="246"/>
       <c r="E35" s="214"/>
       <c r="F35" s="216"/>
       <c r="G35" s="219"/>
       <c r="H35" s="219"/>
-      <c r="I35" s="264"/>
-      <c r="J35" s="265"/>
-      <c r="K35" s="265"/>
+      <c r="I35" s="265"/>
+      <c r="J35" s="266"/>
+      <c r="K35" s="266"/>
       <c r="L35" s="217"/>
-      <c r="M35" s="241" t="s">
+      <c r="M35" s="242" t="s">
         <v>76</v>
       </c>
-      <c r="N35" s="241"/>
+      <c r="N35" s="242"/>
       <c r="P35" s="123"/>
     </row>
     <row r="36" spans="2:16" s="118" customFormat="1" ht="31" x14ac:dyDescent="0.35">
@@ -4163,7 +4172,7 @@
         <f>M37*G37/10^8</f>
         <v>0</v>
       </c>
-      <c r="O37" s="242" t="s">
+      <c r="O37" s="243" t="s">
         <v>77</v>
       </c>
       <c r="P37" s="123"/>
@@ -4194,7 +4203,7 @@
         <f>M38*G38/10^8</f>
         <v>0</v>
       </c>
-      <c r="O38" s="243"/>
+      <c r="O38" s="244"/>
       <c r="P38" s="123"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.35">
@@ -4321,7 +4330,7 @@
       <c r="C47" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="D47" s="152">
+      <c r="D47" s="309">
         <f>(D45+D46)/10^7</f>
         <v>0</v>
       </c>
@@ -4329,7 +4338,7 @@
         <f>SUM(E45:E46)/10^7</f>
         <v>0</v>
       </c>
-      <c r="G47" s="308"/>
+      <c r="G47" s="226"/>
       <c r="P47" s="123"/>
     </row>
     <row r="48" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -4432,14 +4441,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="286" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="237"/>
-      <c r="F1" s="237"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
       <c r="G1" s="108" t="s">
         <v>88</v>
       </c>
@@ -4472,7 +4481,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="267" t="s">
+      <c r="A3" s="300" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="77" t="s">
@@ -4502,7 +4511,7 @@
       <c r="I3" s="94"/>
     </row>
     <row r="4" spans="1:9" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="268"/>
+      <c r="A4" s="301"/>
       <c r="B4" s="77" t="s">
         <v>98</v>
       </c>
@@ -4530,7 +4539,7 @@
       <c r="I4" s="94"/>
     </row>
     <row r="5" spans="1:9" ht="26.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="268"/>
+      <c r="A5" s="301"/>
       <c r="B5" s="77" t="s">
         <v>101</v>
       </c>
@@ -4557,7 +4566,7 @@
       <c r="I5" s="94"/>
     </row>
     <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="268"/>
+      <c r="A6" s="301"/>
       <c r="B6" s="77" t="s">
         <v>102</v>
       </c>
@@ -4575,7 +4584,7 @@
       <c r="H6" s="101"/>
     </row>
     <row r="7" spans="1:9" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="269"/>
+      <c r="A7" s="302"/>
       <c r="B7" s="85" t="s">
         <v>106</v>
       </c>
@@ -4614,14 +4623,14 @@
       <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="284" t="s">
+      <c r="A10" s="267" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="227"/>
-      <c r="C10" s="227"/>
-      <c r="D10" s="227"/>
-      <c r="E10" s="227"/>
-      <c r="F10" s="227"/>
+      <c r="B10" s="228"/>
+      <c r="C10" s="228"/>
+      <c r="D10" s="228"/>
+      <c r="E10" s="228"/>
+      <c r="F10" s="228"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
@@ -4650,7 +4659,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="288" t="s">
+      <c r="A12" s="290" t="s">
         <v>110</v>
       </c>
       <c r="B12" s="74" t="s">
@@ -4679,7 +4688,7 @@
       <c r="I12" s="94"/>
     </row>
     <row r="13" spans="1:9" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="290"/>
+      <c r="A13" s="292"/>
       <c r="B13" s="74" t="s">
         <v>98</v>
       </c>
@@ -4728,14 +4737,14 @@
       <c r="H15" s="63"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="284" t="s">
+      <c r="A16" s="267" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="227"/>
-      <c r="C16" s="227"/>
-      <c r="D16" s="227"/>
-      <c r="E16" s="227"/>
-      <c r="F16" s="227"/>
+      <c r="B16" s="228"/>
+      <c r="C16" s="228"/>
+      <c r="D16" s="228"/>
+      <c r="E16" s="228"/>
+      <c r="F16" s="228"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
@@ -4764,7 +4773,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="288" t="s">
+      <c r="A18" s="290" t="s">
         <v>97</v>
       </c>
       <c r="B18" s="74" t="s">
@@ -4792,7 +4801,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="289"/>
+      <c r="A19" s="291"/>
       <c r="B19" s="74" t="s">
         <v>101</v>
       </c>
@@ -4819,7 +4828,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="289"/>
+      <c r="A20" s="291"/>
       <c r="B20" s="74" t="s">
         <v>113</v>
       </c>
@@ -4841,7 +4850,7 @@
       <c r="H20" s="72"/>
     </row>
     <row r="21" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="289"/>
+      <c r="A21" s="291"/>
       <c r="B21" s="74" t="s">
         <v>114</v>
       </c>
@@ -4863,7 +4872,7 @@
       <c r="H21" s="72"/>
     </row>
     <row r="22" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="289"/>
+      <c r="A22" s="291"/>
       <c r="B22" s="74" t="s">
         <v>115</v>
       </c>
@@ -4885,7 +4894,7 @@
       <c r="H22" s="72"/>
     </row>
     <row r="23" spans="1:8" ht="54.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="290"/>
+      <c r="A23" s="292"/>
       <c r="B23" s="83" t="s">
         <v>116</v>
       </c>
@@ -4923,14 +4932,14 @@
       <c r="H25" s="63"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="284" t="s">
+      <c r="A26" s="267" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="227"/>
-      <c r="C26" s="227"/>
-      <c r="D26" s="227"/>
-      <c r="E26" s="227"/>
-      <c r="F26" s="227"/>
+      <c r="B26" s="228"/>
+      <c r="C26" s="228"/>
+      <c r="D26" s="228"/>
+      <c r="E26" s="228"/>
+      <c r="F26" s="228"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
@@ -4959,7 +4968,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="288" t="s">
+      <c r="A28" s="290" t="s">
         <v>110</v>
       </c>
       <c r="B28" s="74" t="s">
@@ -4987,7 +4996,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="26.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="289"/>
+      <c r="A29" s="291"/>
       <c r="B29" s="74" t="s">
         <v>118</v>
       </c>
@@ -5013,7 +5022,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="289"/>
+      <c r="A30" s="291"/>
       <c r="B30" s="74" t="s">
         <v>113</v>
       </c>
@@ -5035,7 +5044,7 @@
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="289"/>
+      <c r="A31" s="291"/>
       <c r="B31" s="74" t="s">
         <v>114</v>
       </c>
@@ -5057,7 +5066,7 @@
       <c r="H31" s="72"/>
     </row>
     <row r="32" spans="1:8" ht="16.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="290"/>
+      <c r="A32" s="292"/>
       <c r="B32" s="74" t="s">
         <v>115</v>
       </c>
@@ -5104,45 +5113,45 @@
       <c r="A35" s="294" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="237"/>
-      <c r="C35" s="237"/>
-      <c r="D35" s="237"/>
-      <c r="E35" s="238"/>
+      <c r="B35" s="238"/>
+      <c r="C35" s="238"/>
+      <c r="D35" s="238"/>
+      <c r="E35" s="239"/>
       <c r="F35" s="109"/>
       <c r="G35" s="62"/>
       <c r="H35" s="62"/>
     </row>
     <row r="36" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="291" t="s">
+      <c r="A36" s="268" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="291" t="s">
+      <c r="B36" s="268" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="291" t="s">
+      <c r="C36" s="268" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="291" t="s">
+      <c r="D36" s="268" t="s">
         <v>94</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F36" s="301" t="s">
+      <c r="F36" s="282" t="s">
         <v>121</v>
       </c>
       <c r="G36" s="62"/>
       <c r="H36" s="62"/>
     </row>
     <row r="37" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="292"/>
-      <c r="B37" s="292"/>
-      <c r="C37" s="292"/>
-      <c r="D37" s="292"/>
+      <c r="A37" s="269"/>
+      <c r="B37" s="269"/>
+      <c r="C37" s="269"/>
+      <c r="D37" s="269"/>
       <c r="E37" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F37" s="302"/>
+      <c r="F37" s="283"/>
       <c r="G37" s="51"/>
       <c r="H37" s="50" t="s">
         <v>96</v>
@@ -5173,12 +5182,12 @@
       </c>
     </row>
     <row r="39" spans="1:8" s="58" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="296" t="s">
+      <c r="A39" s="297" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="237"/>
-      <c r="C39" s="237"/>
-      <c r="D39" s="237"/>
+      <c r="B39" s="238"/>
+      <c r="C39" s="238"/>
+      <c r="D39" s="238"/>
       <c r="E39" s="9">
         <f>E38</f>
         <v>0.5</v>
@@ -5198,14 +5207,14 @@
       <c r="H40" s="55"/>
     </row>
     <row r="41" spans="1:8" s="54" customFormat="1" ht="21.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="297" t="s">
+      <c r="A41" s="298" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="237"/>
-      <c r="C41" s="237"/>
-      <c r="D41" s="237"/>
-      <c r="E41" s="237"/>
-      <c r="F41" s="237"/>
+      <c r="B41" s="238"/>
+      <c r="C41" s="238"/>
+      <c r="D41" s="238"/>
+      <c r="E41" s="238"/>
+      <c r="F41" s="238"/>
     </row>
     <row r="42" spans="1:8" s="33" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="53" t="s">
@@ -5309,14 +5318,14 @@
       <c r="H46" s="27"/>
     </row>
     <row r="47" spans="1:8" s="26" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="295" t="s">
+      <c r="A47" s="296" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="237"/>
-      <c r="C47" s="237"/>
-      <c r="D47" s="237"/>
-      <c r="E47" s="237"/>
-      <c r="F47" s="237"/>
+      <c r="B47" s="238"/>
+      <c r="C47" s="238"/>
+      <c r="D47" s="238"/>
+      <c r="E47" s="238"/>
+      <c r="F47" s="238"/>
       <c r="G47" s="31"/>
       <c r="H47" s="30">
         <f>SUM(H8,H14,H24,H33,H38,H45)</f>
@@ -5337,35 +5346,35 @@
       <c r="A49" s="293" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="237"/>
-      <c r="C49" s="237"/>
-      <c r="D49" s="237"/>
-      <c r="E49" s="237"/>
-      <c r="F49" s="237"/>
+      <c r="B49" s="238"/>
+      <c r="C49" s="238"/>
+      <c r="D49" s="238"/>
+      <c r="E49" s="238"/>
+      <c r="F49" s="238"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="303" t="s">
+      <c r="A50" s="284" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="304"/>
-      <c r="C50" s="304"/>
-      <c r="D50" s="304"/>
-      <c r="E50" s="304"/>
-      <c r="F50" s="304"/>
+      <c r="B50" s="285"/>
+      <c r="C50" s="285"/>
+      <c r="D50" s="285"/>
+      <c r="E50" s="285"/>
+      <c r="F50" s="285"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="281" t="s">
+      <c r="A51" s="276" t="s">
         <v>136</v>
       </c>
-      <c r="B51" s="280"/>
+      <c r="B51" s="273"/>
       <c r="C51" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="286" t="s">
+      <c r="D51" s="270" t="s">
         <v>137</v>
       </c>
       <c r="E51" s="271"/>
@@ -5379,14 +5388,14 @@
       <c r="A52" s="272" t="s">
         <v>139</v>
       </c>
-      <c r="B52" s="273"/>
-      <c r="C52" s="279" t="s">
+      <c r="B52" s="278"/>
+      <c r="C52" s="287" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="279" t="s">
+      <c r="D52" s="287" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="280"/>
+      <c r="E52" s="273"/>
       <c r="F52" s="23">
         <v>5</v>
       </c>
@@ -5394,10 +5403,10 @@
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="274"/>
-      <c r="B53" s="275"/>
-      <c r="C53" s="287"/>
-      <c r="D53" s="270" t="s">
+      <c r="A53" s="303"/>
+      <c r="B53" s="304"/>
+      <c r="C53" s="288"/>
+      <c r="D53" s="295" t="s">
         <v>142</v>
       </c>
       <c r="E53" s="271"/>
@@ -5408,10 +5417,10 @@
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="276"/>
-      <c r="B54" s="277"/>
-      <c r="C54" s="282"/>
-      <c r="D54" s="270" t="s">
+      <c r="A54" s="280"/>
+      <c r="B54" s="281"/>
+      <c r="C54" s="289"/>
+      <c r="D54" s="295" t="s">
         <v>143</v>
       </c>
       <c r="E54" s="271"/>
@@ -5422,7 +5431,7 @@
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="278" t="s">
+      <c r="A55" s="279" t="s">
         <v>144</v>
       </c>
       <c r="B55" s="271"/>
@@ -5434,17 +5443,17 @@
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="281" t="s">
+      <c r="A56" s="276" t="s">
         <v>136</v>
       </c>
-      <c r="B56" s="280"/>
+      <c r="B56" s="273"/>
       <c r="C56" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D56" s="283" t="s">
+      <c r="D56" s="305" t="s">
         <v>137</v>
       </c>
-      <c r="E56" s="280"/>
+      <c r="E56" s="273"/>
       <c r="F56" s="25" t="s">
         <v>138</v>
       </c>
@@ -5455,14 +5464,14 @@
       <c r="A57" s="272" t="s">
         <v>145</v>
       </c>
-      <c r="B57" s="273"/>
-      <c r="C57" s="279" t="s">
+      <c r="B57" s="278"/>
+      <c r="C57" s="287" t="s">
         <v>146</v>
       </c>
-      <c r="D57" s="279" t="s">
+      <c r="D57" s="287" t="s">
         <v>147</v>
       </c>
-      <c r="E57" s="280"/>
+      <c r="E57" s="273"/>
       <c r="F57" s="23">
         <v>5</v>
       </c>
@@ -5470,13 +5479,13 @@
       <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="276"/>
-      <c r="B58" s="277"/>
-      <c r="C58" s="282"/>
-      <c r="D58" s="279" t="s">
+      <c r="A58" s="280"/>
+      <c r="B58" s="281"/>
+      <c r="C58" s="289"/>
+      <c r="D58" s="287" t="s">
         <v>148</v>
       </c>
-      <c r="E58" s="280"/>
+      <c r="E58" s="273"/>
       <c r="F58" s="23">
         <v>5</v>
       </c>
@@ -5484,7 +5493,7 @@
       <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="278" t="s">
+      <c r="A59" s="279" t="s">
         <v>144</v>
       </c>
       <c r="B59" s="271"/>
@@ -5496,14 +5505,14 @@
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="281" t="s">
+      <c r="A60" s="276" t="s">
         <v>136</v>
       </c>
-      <c r="B60" s="280"/>
+      <c r="B60" s="273"/>
       <c r="C60" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D60" s="286" t="s">
+      <c r="D60" s="270" t="s">
         <v>137</v>
       </c>
       <c r="E60" s="271"/>
@@ -5514,14 +5523,14 @@
       <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="300" t="s">
+      <c r="A61" s="277" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="273"/>
+      <c r="B61" s="278"/>
       <c r="C61" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="D61" s="270" t="s">
+      <c r="D61" s="295" t="s">
         <v>150</v>
       </c>
       <c r="E61" s="271"/>
@@ -5532,7 +5541,7 @@
       <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="278" t="s">
+      <c r="A62" s="279" t="s">
         <v>144</v>
       </c>
       <c r="B62" s="271"/>
@@ -5544,14 +5553,14 @@
       <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="281" t="s">
+      <c r="A63" s="276" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="280"/>
+      <c r="B63" s="273"/>
       <c r="C63" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D63" s="286" t="s">
+      <c r="D63" s="270" t="s">
         <v>137</v>
       </c>
       <c r="E63" s="271"/>
@@ -5565,14 +5574,14 @@
       <c r="A64" s="272" t="s">
         <v>151</v>
       </c>
-      <c r="B64" s="280"/>
+      <c r="B64" s="273"/>
       <c r="C64" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="D64" s="279" t="s">
+      <c r="D64" s="287" t="s">
         <v>152</v>
       </c>
-      <c r="E64" s="280"/>
+      <c r="E64" s="273"/>
       <c r="F64" s="23">
         <v>5</v>
       </c>
@@ -5580,7 +5589,7 @@
       <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="278" t="s">
+      <c r="A65" s="279" t="s">
         <v>144</v>
       </c>
       <c r="B65" s="271"/>
@@ -5592,14 +5601,14 @@
       <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="298" t="s">
+      <c r="A66" s="274" t="s">
         <v>153</v>
       </c>
-      <c r="B66" s="299"/>
-      <c r="C66" s="299"/>
-      <c r="D66" s="299"/>
-      <c r="E66" s="299"/>
-      <c r="F66" s="299"/>
+      <c r="B66" s="275"/>
+      <c r="C66" s="275"/>
+      <c r="D66" s="275"/>
+      <c r="E66" s="275"/>
+      <c r="F66" s="275"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
     </row>
@@ -5608,16 +5617,16 @@
       <c r="H67" s="10"/>
     </row>
     <row r="68" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="266" t="s">
+      <c r="A68" s="299" t="s">
         <v>154</v>
       </c>
-      <c r="B68" s="237"/>
-      <c r="C68" s="237"/>
-      <c r="D68" s="237"/>
-      <c r="E68" s="237"/>
-      <c r="F68" s="237"/>
-      <c r="G68" s="237"/>
-      <c r="H68" s="238"/>
+      <c r="B68" s="238"/>
+      <c r="C68" s="238"/>
+      <c r="D68" s="238"/>
+      <c r="E68" s="238"/>
+      <c r="F68" s="238"/>
+      <c r="G68" s="238"/>
+      <c r="H68" s="239"/>
     </row>
     <row r="69" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="22" t="s">
@@ -5767,20 +5776,22 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A57:B58"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A68:H68"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="A52:B54"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A16:F16"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="C52:C54"/>
@@ -5797,22 +5808,20 @@
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A68:H68"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="A52:B54"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A57:B58"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A50:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -5842,26 +5851,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="306" t="s">
+      <c r="B2" s="307" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="G2" s="307"/>
-      <c r="H2" s="307"/>
-      <c r="I2" s="307"/>
+      <c r="C2" s="308"/>
+      <c r="D2" s="308"/>
+      <c r="E2" s="308"/>
+      <c r="F2" s="308"/>
+      <c r="G2" s="308"/>
+      <c r="H2" s="308"/>
+      <c r="I2" s="308"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="307"/>
-      <c r="C3" s="307"/>
-      <c r="D3" s="307"/>
-      <c r="E3" s="307"/>
-      <c r="F3" s="307"/>
-      <c r="G3" s="307"/>
-      <c r="H3" s="307"/>
-      <c r="I3" s="307"/>
+      <c r="B3" s="308"/>
+      <c r="C3" s="308"/>
+      <c r="D3" s="308"/>
+      <c r="E3" s="308"/>
+      <c r="F3" s="308"/>
+      <c r="G3" s="308"/>
+      <c r="H3" s="308"/>
+      <c r="I3" s="308"/>
     </row>
     <row r="4" spans="2:14" ht="12.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="157"/>
@@ -6050,10 +6059,10 @@
       </c>
       <c r="C13" s="157"/>
       <c r="D13" s="157"/>
-      <c r="E13" s="305" t="s">
+      <c r="E13" s="306" t="s">
         <v>187</v>
       </c>
-      <c r="F13" s="265"/>
+      <c r="F13" s="266"/>
       <c r="G13" s="157"/>
       <c r="H13" s="158"/>
       <c r="I13" s="158"/>

</xml_diff>